<commit_message>
Edit Excel templates. Remove unused templates.  For templates provided to users, (1) format dates according to ISO 8601, and (2) highlight <date issued> in red to indicate required (really the requirement is that at least one child element of originInfo;  dateIssued is a child element of originInfo, so if a spreadsheet has it then the spreadsheet will load fine).
</commit_message>
<xml_diff>
--- a/public/test/metadata_template.xlsx
+++ b/public/test/metadata_template.xlsx
@@ -1,18 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -121,65 +120,45 @@
     <t>location URL</t>
   </si>
   <si>
-    <t> </t>
+    <t/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
-    <numFmt formatCode="GENERAL" numFmtId="164"/>
-    <numFmt formatCode="@" numFmtId="165"/>
-    <numFmt formatCode="@" numFmtId="166"/>
-  </numFmts>
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <charset val="1"/>
-      <family val="2"/>
-      <color rgb="FF000000"/>
-      <sz val="11"/>
     </font>
     <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
+      <b/>
+      <sz val="14"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
-      <name val="Arial"/>
-      <family val="0"/>
+      <b/>
       <sz val="10"/>
-    </font>
-    <font>
       <name val="Calibri"/>
+      <family val="2"/>
       <charset val="1"/>
-      <family val="2"/>
-      <b val="true"/>
-      <color rgb="FF000000"/>
-      <sz val="14"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <charset val="1"/>
-      <family val="2"/>
-      <b val="true"/>
-      <sz val="14"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <charset val="1"/>
-      <family val="2"/>
-      <b val="true"/>
-      <sz val="10"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -204,9 +183,15 @@
         <bgColor rgb="FFF2DCDB"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
-    <border diagonalDown="false" diagonalUp="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -214,89 +199,29 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="41"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="4" numFmtId="166" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="5" numFmtId="166" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="166" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="166" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="3" fontId="5" numFmtId="166" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="4" fontId="5" numFmtId="166" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="4" fontId="4" numFmtId="166" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="165" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="6" numFmtId="165" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
+  <cellXfs count="13">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
-    <cellStyle builtinId="3" customBuiltin="false" name="Comma" xfId="15"/>
-    <cellStyle builtinId="6" customBuiltin="false" name="Comma [0]" xfId="16"/>
-    <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
-    <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
-    <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -355,66 +280,360 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="1:3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AMJ3"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="I1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="L9" activeCellId="0" pane="topLeft" sqref="L9"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="U1" sqref="U1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="19.004048582996"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="25.8502024291498"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="20.2793522267206"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="13.9959514170041"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="23"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="29.1417004048583"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="9.21862348178138"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="38.4251012145749"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="24.2793522267206"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="9.21862348178138"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="23.8178137651822"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="23.5748987854251"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="9.74089068825911"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="27.5708502024291"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="14.9959514170041"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="23.5748987854251"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="31.5708502024291"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="22.7085020242915"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="19.5748987854251"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="1" width="18.1376518218623"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="1" width="30.8582995951417"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="17.4251012145749"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="1" width="20.004048582996"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="20.1376518218623"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="1" width="27.1457489878542"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="1" width="32.7125506072874"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="1" width="25"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="1" width="26.1457489878542"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="1" width="23.1457489878542"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="1" width="23.4251012145749"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="1" width="24"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="1" width="12.7125506072875"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="1" width="9.1417004048583"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="1" width="13.7125506072874"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="1" width="22.4251012145749"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="1" width="23.8502024291498"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="1" width="22.2793522267206"/>
-    <col collapsed="false" hidden="false" max="1023" min="38" style="1" width="9.1417004048583"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="9.1417004048583"/>
+    <col min="1" max="1" width="19" style="1"/>
+    <col min="2" max="2" width="25.85546875" style="1"/>
+    <col min="3" max="3" width="20.28515625" style="1"/>
+    <col min="4" max="4" width="14" style="1"/>
+    <col min="5" max="5" width="23" style="1"/>
+    <col min="6" max="6" width="29.140625" style="1"/>
+    <col min="7" max="7" width="9.140625" style="1"/>
+    <col min="8" max="8" width="38.42578125" style="1"/>
+    <col min="9" max="9" width="24.28515625" style="1"/>
+    <col min="10" max="10" width="9.140625" style="1"/>
+    <col min="11" max="11" width="23.85546875" style="1"/>
+    <col min="12" max="12" width="23.5703125" style="1"/>
+    <col min="13" max="13" width="9.7109375" style="1"/>
+    <col min="14" max="14" width="27.5703125" style="1"/>
+    <col min="15" max="15" width="15" style="1"/>
+    <col min="16" max="16" width="23.5703125" style="1"/>
+    <col min="17" max="17" width="31.5703125" style="1"/>
+    <col min="18" max="18" width="22.7109375" style="1"/>
+    <col min="19" max="19" width="19.5703125" style="1"/>
+    <col min="20" max="20" width="18.140625" style="1"/>
+    <col min="21" max="21" width="30.85546875" style="1"/>
+    <col min="22" max="22" width="17.42578125" style="1"/>
+    <col min="23" max="23" width="20" style="1"/>
+    <col min="24" max="24" width="20.140625" style="1"/>
+    <col min="25" max="25" width="27.140625" style="1"/>
+    <col min="26" max="26" width="32.7109375" style="1"/>
+    <col min="27" max="27" width="25" style="1"/>
+    <col min="28" max="28" width="26.140625" style="1"/>
+    <col min="29" max="29" width="23.140625" style="1"/>
+    <col min="30" max="30" width="23.42578125" style="1"/>
+    <col min="31" max="31" width="24" style="1"/>
+    <col min="32" max="32" width="12.7109375" style="1"/>
+    <col min="33" max="33" width="9.140625" style="1"/>
+    <col min="34" max="34" width="13.7109375" style="1"/>
+    <col min="35" max="35" width="22.42578125" style="1"/>
+    <col min="36" max="36" width="23.85546875" style="1"/>
+    <col min="37" max="37" width="22.28515625" style="1"/>
+    <col min="38" max="1023" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="17.9" outlineLevel="0" r="1" s="9">
+    <row r="1" spans="1:1024" s="9" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -469,7 +688,7 @@
       <c r="R1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="S1" s="12" t="s">
         <v>16</v>
       </c>
       <c r="T1" s="4" t="s">
@@ -526,77 +745,52 @@
       <c r="AK1" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="AMJ1" s="0"/>
+      <c r="AMJ1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="2">
+    <row r="2" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>34</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="3">
+    <row r="3" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>34</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.5748987854251"/>
+    <col min="1" max="1025" width="8.5703125"/>
   </cols>
   <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.5748987854251"/>
+    <col min="1" max="1025" width="8.5703125"/>
   </cols>
   <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>